<commit_message>
Updated design proposal Q3
</commit_message>
<xml_diff>
--- a/Sense_Costing.xlsx
+++ b/Sense_Costing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\portm\Documents\University\2023F\EEE3088F\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\portm\Documents\GitHub\EEE3088F_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82735C0A-DDB5-4C9F-B09C-F82D61478743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE92915-145E-4C3F-A253-3FB1D52CD33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2070" windowWidth="29040" windowHeight="15720" xr2:uid="{71D04402-5253-46E2-AF73-2214C38D2B17}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Part Num</t>
   </si>
@@ -81,9 +80,6 @@
     <t>0805W8F1002T5E</t>
   </si>
   <si>
-    <t>Part</t>
-  </si>
-  <si>
     <t>Package</t>
   </si>
   <si>
@@ -103,13 +99,25 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Part Description</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>IC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,9 +126,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Microsoft YaHei"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -132,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,14 +161,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,198 +505,390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D929545-741B-4B22-B1F2-F9B41A0F9C91}">
-  <dimension ref="B4:J17"/>
+  <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T28" sqref="O17:T28"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="I5" s="4">
+        <f>F5*H5+G5*3</f>
+        <v>3.52</v>
+      </c>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.38869999999999999</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" ref="I6:I16" si="0">F6*H6+G6*3</f>
+        <v>3.7774000000000001</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4">
         <v>6</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0.13</v>
-      </c>
-      <c r="G5">
-        <f>D5*F5+E5*3</f>
-        <v>3.52</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0.38869999999999999</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ref="G6:G16" si="0">D6*F6+E6*3</f>
-        <v>3.7774000000000001</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1E-3</v>
-      </c>
-      <c r="G7">
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I8" s="4">
         <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17">
-        <f>SUM(G5:G16)</f>
+      <c r="I17" s="2">
+        <f>SUM(I5:I16)</f>
         <v>7.3033999999999999</v>
       </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>